<commit_message>
added calculation for new use case 'Music'
</commit_message>
<xml_diff>
--- a/FunctionPoints/CalculationFunctionPoints.xlsx
+++ b/FunctionPoints/CalculationFunctionPoints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Use Case</t>
   </si>
@@ -50,18 +50,18 @@
     <t>Create Event</t>
   </si>
   <si>
+    <t>Date time</t>
+  </si>
+  <si>
+    <t>Playlist</t>
+  </si>
+  <si>
     <t>Song</t>
   </si>
   <si>
-    <t>Playlist</t>
-  </si>
-  <si>
     <t>Communication</t>
   </si>
   <si>
-    <t>Date time</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Function Points wurden gebildet aus den "Sub-Tasks" in Jira der einzelnen Use-Cases</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -455,960 +458,6 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Function Points </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>/ Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="4"/>
-            <c:backward val="4"/>
-            <c:intercept val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7EDD-4A6E-98B5-CE075D2F717D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-272579168"/>
-        <c:axId val="-272588960"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-272579168"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Time in h</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-272588960"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-272588960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Function Points</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-272579168"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
@@ -1520,10 +569,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$9:$C$13</c:f>
+              <c:f>Sheet2!$C$9:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.8766917293233083</c:v>
                 </c:pt>
@@ -1539,15 +588,18 @@
                 <c:pt idx="4">
                   <c:v>9.2390977443609028</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.538345864661654</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$G$9:$G$13</c:f>
+              <c:f>Sheet2!$G$9:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13</c:v>
                 </c:pt>
@@ -1563,10 +615,18 @@
                 <c:pt idx="4">
                   <c:v>64</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59C1-48D1-B2BB-B8EEBFA7569A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -1636,6 +696,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-59C1-48D1-B2BB-B8EEBFA7569A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1645,11 +710,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-272585696"/>
-        <c:axId val="-272583520"/>
+        <c:axId val="213176096"/>
+        <c:axId val="213165760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-272585696"/>
+        <c:axId val="213176096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1763,12 +828,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-272583520"/>
+        <c:crossAx val="213165760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-272583520"/>
+        <c:axId val="213165760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,7 +946,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-272585696"/>
+        <c:crossAx val="213176096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1970,46 +1035,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2526,579 +1551,27 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>583095</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>101876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>468795</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>101876</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2024743</xdr:colOff>
+      <xdr:colOff>2019300</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>81642</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Diagramm 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3112,7 +1585,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3167,8 +1640,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B8:H13" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7" dataCellStyle="Akzent5">
-  <autoFilter ref="B8:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="B8:H14" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7" dataCellStyle="Akzent5">
+  <autoFilter ref="B8:H14"/>
   <sortState ref="B9:H13">
     <sortCondition ref="G8:G13"/>
   </sortState>
@@ -3761,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3930,7 +2403,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <f>G9/Tabelle1[[#Totals],[FPC / Time]]</f>
@@ -3946,11 +2419,11 @@
         <v>5</v>
       </c>
       <c r="G9" s="1">
-        <f>E9*D9+F9</f>
+        <f t="shared" ref="G9:G14" si="0">E9*D9+F9</f>
         <v>13</v>
       </c>
       <c r="H9" s="2">
-        <f>G9/C9</f>
+        <f t="shared" ref="H9:H14" si="1">G9/C9</f>
         <v>6.927083333333333</v>
       </c>
     </row>
@@ -3972,11 +2445,11 @@
         <v>3</v>
       </c>
       <c r="G10" s="1">
-        <f>E10*D10+F10</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H10" s="2">
-        <f>G10/C10</f>
+        <f t="shared" si="1"/>
         <v>6.927083333333333</v>
       </c>
     </row>
@@ -3998,17 +2471,17 @@
         <v>7</v>
       </c>
       <c r="G11" s="1">
-        <f>E11*D11+F11</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="H11" s="2">
-        <f>G11/C11</f>
+        <f t="shared" si="1"/>
         <v>6.927083333333333</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
         <f>G12/Tabelle1[[#Totals],[FPC / Time]]</f>
@@ -4024,17 +2497,17 @@
         <v>5</v>
       </c>
       <c r="G12" s="1">
-        <f>E12*D12+F12</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="H12" s="2">
-        <f>G12/C12</f>
+        <f t="shared" si="1"/>
         <v>6.927083333333333</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
         <f>G13/Tabelle1[[#Totals],[FPC / Time]]</f>
@@ -4050,12 +2523,38 @@
         <v>8</v>
       </c>
       <c r="G13" s="1">
-        <f>E13*D13+F13</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="H13" s="2">
-        <f>G13/C13</f>
+        <f t="shared" si="1"/>
         <v>6.927083333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <f>G14/Tabelle1[[#Totals],[FPC / Time]]</f>
+        <v>10.538345864661654</v>
+      </c>
+      <c r="D14" s="1">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9270833333333339</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>